<commit_message>
1.Translated into Albanian language  the  full sentences  of the MECO datasets reading task.
</commit_message>
<xml_diff>
--- a/datasets/MECO-dataset/release 1.0/auxiliary files/reading task materials/supp texts.xlsx
+++ b/datasets/MECO-dataset/release 1.0/auxiliary files/reading task materials/supp texts.xlsx
@@ -1,15 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145A4665-3D0E-4187-AB8F-34169D0E9937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB5E434-1615-4628-9DDC-26804C5E4ADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$3:$O$3</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <si>
     <t>Dutch</t>
   </si>
@@ -563,6 +566,12 @@
   </si>
   <si>
     <t>Shaka märki seostatakse üldiselt Havai ja surfamisega. Žesti moodustamiseks sirutatakse käel välja väike sõrm ja pöial ning muud sõrmed surutakse samal ajal rusikasse kokku. Käelaba võib olla suunatud nii ettepoole kui ka tahapoole. Kuuekümnendatel võtsid kohalikelt havailastelt shaka žesti üle surfarid, ja see žest levis üle kogu maailma. Žest on samuti levinud langevarjuhüppajate, sukeldujate, pilootide, rulasõitjate ja kiirlendurite hulgas. Märki kasutatakse põhiliselt tervituse ning tänu või tunnustuse väljendamiseks. Kohalikud havailased kasutavad shaka märki, et edasi anda “aloha” vaimu, mis hõlmab endast sõprust, üksteise mõistmist, solidaarsust erinevate etniliste kultuuride vahel, kes Havail elavad. Märgi täpne päritolu on ebaselge, kuid on välja pakutud, et märk on pärit hispaania immigrantidelt, kes surusid keskmised sõrmed kokku ja tõid pöidlad huulte juurde, et illustreerida ühist joomingut kohalikega, keda nad Havail kohtasid. Ameerika viipekeeles märgib shaka žest verbi mängima.</t>
+  </si>
+  <si>
+    <t>Albanian</t>
+  </si>
+  <si>
+    <t>Në fenë dhe mitin e lashtë romak, Janusi është perëndia e fillimeve dhe portave. Ai ka një natyrë të dyfishtë dhe zakonisht përshkruhet si me dy fytyra, pasi shikon drejt së ardhmes dhe të kaluarës. Janusi kryesonte fillimin dhe mbarimin e konfliktit, dhe për rrjedhojë luftën dhe paqen. Dyert e tempullit të tij ishin të hapura në kohë lufte dhe të mbyllura gjatë kohës së paqes. Si perëndia e portave, ai shoqërohej gjithashtu me hyrjen dhe daljen nga dyert e shtëpive. Janusi shpesh simbolizonte ndryshimin dhe tranzicionet, të tilla si përparimi nga një gjendje në tjetrën, nga një vizion në tjetrin dhe rritja e të rinjve në moshë madhore. Prandaj, Janusi adhurohej në fillim të kohës së korrjes dhe mbjelljes, si dhe në martesa, vdekje dhe fillime të tjera. Janusi nuk kishte një prift të specializuar të caktuar për të, por vetë kryeprifti kryente ceremonitë e tij. Janusi përfaqësonte terrenin e mesëm midis barbarizmit dhe qytetërimit, hapësirës rurale dhe urbane, rinisë dhe moshës madhore. Grekët e lashtë nuk kishin ekuivalent me Janusin, të cilin romakët e pretendonin si të tyren.</t>
   </si>
 </sst>
 </file>
@@ -573,21 +582,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="1"/>
       <scheme val="major"/>
     </font>
@@ -620,16 +629,16 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -915,21 +924,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="11" width="10.58203125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="12" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.58203125" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.6640625" style="1"/>
+    <col min="1" max="1" width="8.6328125" style="1"/>
+    <col min="2" max="13" width="255.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.6328125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="70" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
@@ -968,7 +975,7 @@
       </c>
       <c r="O1" s="3"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1017,7 @@
       </c>
       <c r="O2" s="3"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -1052,7 +1059,7 @@
       </c>
       <c r="O3" s="3"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>168</v>
       </c>
@@ -1094,7 +1101,7 @@
       </c>
       <c r="O4" s="3"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -1136,7 +1143,7 @@
       </c>
       <c r="O5" s="3"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1178,7 +1185,7 @@
       </c>
       <c r="O6" s="3"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1220,7 +1227,7 @@
       </c>
       <c r="O7" s="3"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1262,7 +1269,7 @@
       </c>
       <c r="O8" s="3"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1304,7 +1311,7 @@
       </c>
       <c r="O9" s="3"/>
     </row>
-    <row r="10" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -1346,7 +1353,7 @@
       </c>
       <c r="O10" s="3"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" ht="26" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -1388,7 +1395,7 @@
       </c>
       <c r="O11" s="3"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1430,7 +1437,7 @@
       </c>
       <c r="O12" s="3"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>10</v>
       </c>
@@ -1472,7 +1479,7 @@
       </c>
       <c r="O13" s="3"/>
     </row>
-    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>11</v>
       </c>
@@ -1514,40 +1521,47 @@
       </c>
       <c r="O14" s="3"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="O15" s="3"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="15:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="15:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="15:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="15:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="15:15" x14ac:dyDescent="0.35">
       <c r="O25" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A3:O3" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>